<commit_message>
Add folder without nested Git repository
</commit_message>
<xml_diff>
--- a/static/EC Modello.xlsx
+++ b/static/EC Modello.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isabellaferrero/Politecnico Di Torino Studenti Dropbox/Isabella Ferrero/Mac/Desktop/EC processor versions/desktop EC processor/static/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mgazzino\Desktop\CODES\EC processor v1.0\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8BCB55A-18B9-1E4D-9BB2-77BD0028087E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC45DA8D-A68D-4B77-A484-13629E335D0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SCHEDE" sheetId="1" r:id="rId1"/>
@@ -364,7 +364,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="49">
+  <borders count="63">
     <border>
       <left/>
       <right/>
@@ -835,21 +835,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color theme="6"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top style="thin">
         <color indexed="64"/>
@@ -936,6 +921,201 @@
         <color theme="9" tint="-0.249977111117893"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="thin">
+        <color theme="6"/>
+      </top>
+      <bottom style="thin">
+        <color theme="6"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="thin">
+        <color theme="6"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="6"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="thin">
+        <color theme="6"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="thin">
+        <color theme="6"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="6"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="thin">
+        <color theme="6"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="6"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="6"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFFF0000"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -944,7 +1124,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="121">
+  <cellXfs count="130">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1043,151 +1223,8 @@
     <xf numFmtId="44" fontId="8" fillId="9" borderId="20" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="10" borderId="28" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="11" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="6" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="12" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="13" borderId="28" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="13" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="14" borderId="28" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="4" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="36" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="3" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="11" fillId="15" borderId="39" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="6" borderId="39" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="39" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="13" borderId="36" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="13" borderId="38" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="36" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="38" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1195,26 +1232,209 @@
     <xf numFmtId="0" fontId="5" fillId="12" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="44" fontId="5" fillId="2" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="2" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="5" fillId="2" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="10" fontId="5" fillId="2" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="2" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="7" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="2" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="36" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="10" borderId="28" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="2" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="3" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="11" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="11" fillId="15" borderId="39" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="6" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="7" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="39" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="12" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="13" borderId="28" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="13" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="14" borderId="28" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -1230,7 +1450,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1257,6 +1477,46 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="53" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="54" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="13" borderId="57" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="13" borderId="58" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="13" borderId="59" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="13" borderId="60" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="57" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="58" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="61" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="62" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2059,249 +2319,251 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="21.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="21.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="41"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="42" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="48" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="49"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="51"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="44"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="42" t="s">
+      <c r="B2" s="53"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="55"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="44"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="42" t="s">
+      <c r="B3" s="117"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="55"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="46" t="e">
+      <c r="B4" s="56" t="e">
         <f>D21</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="44"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="47"/>
-      <c r="B5" s="48"/>
-      <c r="C5" s="48"/>
-      <c r="D5" s="49"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="50"/>
-      <c r="B6" s="75" t="s">
+      <c r="C4" s="54"/>
+      <c r="D4" s="55"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="57"/>
+      <c r="B5" s="58"/>
+      <c r="C5" s="58"/>
+      <c r="D5" s="59"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="60"/>
+      <c r="B6" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="75" t="s">
+      <c r="C6" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="51" t="s">
+      <c r="D6" s="62" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="52" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="76"/>
-      <c r="C7" s="76"/>
-      <c r="D7" s="53">
+      <c r="B7" s="64"/>
+      <c r="C7" s="64"/>
+      <c r="D7" s="65">
         <f>B7+C7</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="42" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="77">
+      <c r="B8" s="66">
         <f>B7/25</f>
         <v>0</v>
       </c>
-      <c r="C8" s="88"/>
-      <c r="D8" s="54"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="55" t="s">
+      <c r="C8" s="67"/>
+      <c r="D8" s="68"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="78">
+      <c r="B9" s="70">
         <f>B8*B3</f>
         <v>0</v>
       </c>
-      <c r="C9" s="78">
+      <c r="C9" s="70">
         <f>C7</f>
         <v>0</v>
       </c>
-      <c r="D9" s="56">
+      <c r="D9" s="71">
         <f>C9+B9</f>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="57"/>
-      <c r="B10" s="79"/>
-      <c r="C10" s="79"/>
-      <c r="D10" s="58"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="59" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="72"/>
+      <c r="B10" s="73"/>
+      <c r="C10" s="73"/>
+      <c r="D10" s="74"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="80" t="s">
+      <c r="B11" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="80" t="s">
+      <c r="C11" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="60"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="61"/>
-      <c r="B12" s="81"/>
-      <c r="C12" s="81"/>
-      <c r="D12" s="54"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="59" t="s">
+      <c r="D11" s="77"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="78"/>
+      <c r="B12" s="47"/>
+      <c r="C12" s="47"/>
+      <c r="D12" s="68"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="82"/>
-      <c r="C13" s="82"/>
-      <c r="D13" s="60">
+      <c r="B13" s="79"/>
+      <c r="C13" s="79"/>
+      <c r="D13" s="77">
         <f>B13+C13</f>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="61"/>
-      <c r="B14" s="81"/>
-      <c r="C14" s="81"/>
-      <c r="D14" s="54"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="62" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="78"/>
+      <c r="B14" s="47"/>
+      <c r="C14" s="47"/>
+      <c r="D14" s="68"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="88" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="83" t="e">
+      <c r="B15" s="118" t="e">
         <f>B7*(1+B11)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C15" s="83" t="e">
+      <c r="C15" s="119" t="e">
         <f>C7*(1+C11)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="D15" s="63" t="e">
+      <c r="D15" s="80" t="e">
         <f>B15+C15</f>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="61"/>
-      <c r="B16" s="81"/>
-      <c r="C16" s="81"/>
-      <c r="D16" s="54"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="64" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="89"/>
+      <c r="B16" s="120"/>
+      <c r="C16" s="121"/>
+      <c r="D16" s="68"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="90" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="84" t="e">
+      <c r="B17" s="122" t="e">
         <f>B15-B7</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C17" s="84" t="e">
+      <c r="C17" s="123" t="e">
         <f>C15-C7</f>
         <v>#VALUE!</v>
       </c>
-      <c r="D17" s="65" t="e">
+      <c r="D17" s="81" t="e">
         <f>D15-D7</f>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="66" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="91" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="85" t="e">
+      <c r="B18" s="124" t="e">
         <f>(B15-B7)/B7</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C18" s="85" t="e">
+      <c r="C18" s="125" t="e">
         <f>(C15-C7)/C7</f>
         <v>#VALUE!</v>
       </c>
-      <c r="D18" s="67" t="e">
+      <c r="D18" s="82" t="e">
         <f>(D15-D7)/D7</f>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="61"/>
-      <c r="B19" s="81"/>
-      <c r="C19" s="81"/>
-      <c r="D19" s="68"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="69" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="89"/>
+      <c r="B19" s="120"/>
+      <c r="C19" s="121"/>
+      <c r="D19" s="83"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="92" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="86" t="e">
+      <c r="B20" s="126" t="e">
         <f>B15-(B8*65)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C20" s="86" t="e">
+      <c r="C20" s="127" t="e">
         <f>C15-C7</f>
         <v>#VALUE!</v>
       </c>
-      <c r="D20" s="70" t="e">
+      <c r="D20" s="84" t="e">
         <f>D15-D9</f>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="71" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="93" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="87" t="e">
+      <c r="B21" s="128" t="e">
         <f>(B20-B9)/B9</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C21" s="87" t="e">
+      <c r="C21" s="129" t="e">
         <f>(C20-C9)/C9</f>
         <v>#VALUE!</v>
       </c>
-      <c r="D21" s="72" t="e">
+      <c r="D21" s="85" t="e">
         <f>(D15-D9)/D9</f>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="73"/>
-      <c r="B22" s="89"/>
-      <c r="C22" s="89"/>
-      <c r="D22" s="74"/>
+    <row r="22" spans="1:4" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="86"/>
+      <c r="B22" s="94"/>
+      <c r="C22" s="94"/>
+      <c r="D22" s="87"/>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="9clA0nCuLeZtLml6QNMUXTdEvedWL/8gJt7WrtsYhw3uhA750YMKfREjbeGvILtX3orOoI7l9e6uHjbGxru/SA==" saltValue="uf9EUGnpCRotUaiFggHvjg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2313,113 +2575,113 @@
       <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="9" width="13.6640625" customWidth="1"/>
-    <col min="10" max="10" width="8.83203125" customWidth="1"/>
-    <col min="11" max="11" width="9.1640625" customWidth="1"/>
-    <col min="12" max="13" width="7.6640625" customWidth="1"/>
-    <col min="14" max="14" width="6.83203125" customWidth="1"/>
-    <col min="15" max="15" width="8.1640625" style="8" customWidth="1"/>
-    <col min="16" max="16" width="14.6640625" customWidth="1"/>
-    <col min="17" max="17" width="13.6640625" customWidth="1"/>
-    <col min="18" max="18" width="7.33203125" customWidth="1"/>
+    <col min="1" max="9" width="13.625" customWidth="1"/>
+    <col min="10" max="10" width="8.875" customWidth="1"/>
+    <col min="11" max="11" width="9.125" customWidth="1"/>
+    <col min="12" max="13" width="7.625" customWidth="1"/>
+    <col min="14" max="14" width="6.875" customWidth="1"/>
+    <col min="15" max="15" width="8.125" style="8" customWidth="1"/>
+    <col min="16" max="16" width="14.625" customWidth="1"/>
+    <col min="17" max="17" width="13.625" customWidth="1"/>
+    <col min="18" max="18" width="7.375" customWidth="1"/>
     <col min="19" max="19" width="6.5" style="1" customWidth="1"/>
-    <col min="20" max="21" width="9.33203125" customWidth="1"/>
+    <col min="20" max="21" width="9.375" customWidth="1"/>
     <col min="22" max="22" width="12" customWidth="1"/>
     <col min="23" max="23" width="12.5" customWidth="1"/>
-    <col min="24" max="25" width="8.83203125" customWidth="1"/>
-    <col min="26" max="26" width="11.33203125" style="11" customWidth="1"/>
+    <col min="24" max="25" width="8.875" customWidth="1"/>
+    <col min="26" max="26" width="11.375" style="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="N1" s="111" t="s">
+    <row r="1" spans="1:26" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N1" s="107" t="s">
         <v>18</v>
       </c>
-      <c r="O1" s="100"/>
-      <c r="P1" s="100"/>
-      <c r="Q1" s="100"/>
-      <c r="R1" s="99" t="s">
+      <c r="O1" s="96"/>
+      <c r="P1" s="96"/>
+      <c r="Q1" s="96"/>
+      <c r="R1" s="95" t="s">
         <v>19</v>
       </c>
-      <c r="S1" s="100"/>
-      <c r="T1" s="100"/>
-      <c r="U1" s="100"/>
-      <c r="V1" s="100"/>
-      <c r="W1" s="100"/>
-      <c r="X1" s="100"/>
-      <c r="Y1" s="100"/>
-      <c r="Z1" s="101"/>
-    </row>
-    <row r="2" spans="1:26" s="1" customFormat="1" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="N2" s="112"/>
-      <c r="O2" s="103"/>
-      <c r="P2" s="103"/>
-      <c r="Q2" s="103"/>
-      <c r="R2" s="102"/>
-      <c r="S2" s="103"/>
-      <c r="T2" s="103"/>
-      <c r="U2" s="103"/>
-      <c r="V2" s="103"/>
-      <c r="W2" s="103"/>
-      <c r="X2" s="103"/>
-      <c r="Y2" s="103"/>
-      <c r="Z2" s="104"/>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="N3" s="113" t="s">
+      <c r="S1" s="96"/>
+      <c r="T1" s="96"/>
+      <c r="U1" s="96"/>
+      <c r="V1" s="96"/>
+      <c r="W1" s="96"/>
+      <c r="X1" s="96"/>
+      <c r="Y1" s="96"/>
+      <c r="Z1" s="97"/>
+    </row>
+    <row r="2" spans="1:26" s="1" customFormat="1" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="N2" s="108"/>
+      <c r="O2" s="99"/>
+      <c r="P2" s="99"/>
+      <c r="Q2" s="99"/>
+      <c r="R2" s="98"/>
+      <c r="S2" s="99"/>
+      <c r="T2" s="99"/>
+      <c r="U2" s="99"/>
+      <c r="V2" s="99"/>
+      <c r="W2" s="99"/>
+      <c r="X2" s="99"/>
+      <c r="Y2" s="99"/>
+      <c r="Z2" s="100"/>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="N3" s="109" t="s">
         <v>20</v>
       </c>
-      <c r="O3" s="114"/>
-      <c r="P3" s="114"/>
-      <c r="Q3" s="115"/>
-      <c r="R3" s="102"/>
-      <c r="S3" s="103"/>
-      <c r="T3" s="105"/>
-      <c r="U3" s="105"/>
-      <c r="V3" s="105"/>
-      <c r="W3" s="105"/>
-      <c r="X3" s="105"/>
-      <c r="Y3" s="105"/>
-      <c r="Z3" s="104"/>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="N4" s="116" t="s">
+      <c r="O3" s="110"/>
+      <c r="P3" s="110"/>
+      <c r="Q3" s="111"/>
+      <c r="R3" s="98"/>
+      <c r="S3" s="99"/>
+      <c r="T3" s="101"/>
+      <c r="U3" s="101"/>
+      <c r="V3" s="101"/>
+      <c r="W3" s="101"/>
+      <c r="X3" s="101"/>
+      <c r="Y3" s="101"/>
+      <c r="Z3" s="100"/>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="N4" s="112" t="s">
         <v>21</v>
       </c>
-      <c r="O4" s="114"/>
+      <c r="O4" s="110"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="3">
         <f ca="1">TODAY()</f>
-        <v>45632</v>
-      </c>
-      <c r="R4" s="102"/>
-      <c r="S4" s="103"/>
-      <c r="T4" s="105"/>
-      <c r="U4" s="105"/>
-      <c r="V4" s="105"/>
-      <c r="W4" s="105"/>
-      <c r="X4" s="105"/>
-      <c r="Y4" s="105"/>
-      <c r="Z4" s="104"/>
-    </row>
-    <row r="5" spans="1:26" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>45701</v>
+      </c>
+      <c r="R4" s="98"/>
+      <c r="S4" s="99"/>
+      <c r="T4" s="101"/>
+      <c r="U4" s="101"/>
+      <c r="V4" s="101"/>
+      <c r="W4" s="101"/>
+      <c r="X4" s="101"/>
+      <c r="Y4" s="101"/>
+      <c r="Z4" s="100"/>
+    </row>
+    <row r="5" spans="1:26" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K5" s="4"/>
       <c r="N5" s="5"/>
       <c r="O5" s="6"/>
       <c r="P5" s="7"/>
       <c r="Q5" s="7"/>
-      <c r="R5" s="106"/>
-      <c r="S5" s="107"/>
-      <c r="T5" s="107"/>
-      <c r="U5" s="107"/>
-      <c r="V5" s="107"/>
-      <c r="W5" s="107"/>
-      <c r="X5" s="107"/>
-      <c r="Y5" s="107"/>
-      <c r="Z5" s="108"/>
-    </row>
-    <row r="6" spans="1:26" ht="17" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="R5" s="102"/>
+      <c r="S5" s="103"/>
+      <c r="T5" s="103"/>
+      <c r="U5" s="103"/>
+      <c r="V5" s="103"/>
+      <c r="W5" s="103"/>
+      <c r="X5" s="103"/>
+      <c r="Y5" s="103"/>
+      <c r="Z5" s="104"/>
+    </row>
+    <row r="6" spans="1:26" ht="17.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="K6" s="4"/>
       <c r="R6" s="9"/>
       <c r="S6" s="9"/>
@@ -2431,35 +2693,35 @@
       <c r="Y6" s="9"/>
       <c r="Z6" s="9"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="K7" s="10"/>
     </row>
-    <row r="8" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="90" t="s">
+    <row r="8" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="91" t="s">
+      <c r="B8" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="91" t="s">
+      <c r="C8" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="91" t="s">
+      <c r="D8" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="E8" s="91" t="s">
+      <c r="E8" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="F8" s="91" t="s">
+      <c r="F8" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="G8" s="91" t="s">
+      <c r="G8" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="H8" s="92" t="s">
+      <c r="H8" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="I8" s="91" t="s">
+      <c r="I8" s="39" t="s">
         <v>44</v>
       </c>
       <c r="K8" s="12" t="s">
@@ -2474,10 +2736,10 @@
       <c r="N8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="O8" s="117" t="s">
-        <v>25</v>
-      </c>
-      <c r="P8" s="118"/>
+      <c r="O8" s="113" t="s">
+        <v>25</v>
+      </c>
+      <c r="P8" s="114"/>
       <c r="Q8" s="15" t="s">
         <v>26</v>
       </c>
@@ -2509,40 +2771,40 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A9" s="98">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A9" s="46">
         <f>SCHEDE!B1</f>
         <v>0</v>
       </c>
-      <c r="B9" s="93">
+      <c r="B9" s="41">
         <f>SCHEDE!D7</f>
         <v>0</v>
       </c>
-      <c r="C9" s="93">
+      <c r="C9" s="41">
         <f>SCHEDE!D9</f>
         <v>0</v>
       </c>
-      <c r="D9" s="93">
+      <c r="D9" s="41">
         <f>SCHEDE!D13</f>
         <v>0</v>
       </c>
-      <c r="E9" s="93" t="e">
+      <c r="E9" s="41" t="e">
         <f>SCHEDE!B15</f>
         <v>#VALUE!</v>
       </c>
-      <c r="F9" s="97" t="e">
+      <c r="F9" s="45" t="e">
         <f>SCHEDE!C15</f>
         <v>#VALUE!</v>
       </c>
-      <c r="G9" s="94" t="str">
+      <c r="G9" s="42" t="str">
         <f>SCHEDE!C11</f>
         <v>--</v>
       </c>
-      <c r="H9" s="95" t="e">
+      <c r="H9" s="43" t="e">
         <f>SCHEDE!D15</f>
         <v>#VALUE!</v>
       </c>
-      <c r="I9" s="96">
+      <c r="I9" s="44">
         <f>SCHEDE!B8</f>
         <v>0</v>
       </c>
@@ -2550,8 +2812,8 @@
       <c r="L9" s="19"/>
       <c r="M9" s="19"/>
       <c r="N9" s="19"/>
-      <c r="O9" s="109"/>
-      <c r="P9" s="110"/>
+      <c r="O9" s="105"/>
+      <c r="P9" s="106"/>
       <c r="Q9" s="18"/>
       <c r="R9" s="20"/>
       <c r="S9" s="20">
@@ -2582,40 +2844,40 @@
       </c>
       <c r="Z9" s="25"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A10" s="98">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A10" s="46">
         <f>SCHEDE!B24</f>
         <v>0</v>
       </c>
-      <c r="B10" s="93">
+      <c r="B10" s="41">
         <f>SCHEDE!D30</f>
         <v>0</v>
       </c>
-      <c r="C10" s="93">
+      <c r="C10" s="41">
         <f>SCHEDE!D32</f>
         <v>0</v>
       </c>
-      <c r="D10" s="93">
+      <c r="D10" s="41">
         <f>SCHEDE!D36</f>
         <v>0</v>
       </c>
-      <c r="E10" s="93">
+      <c r="E10" s="41">
         <f>SCHEDE!B38</f>
         <v>0</v>
       </c>
-      <c r="F10" s="97">
+      <c r="F10" s="45">
         <f>SCHEDE!C38</f>
         <v>0</v>
       </c>
-      <c r="G10" s="94">
+      <c r="G10" s="42">
         <f>SCHEDE!C34</f>
         <v>0</v>
       </c>
-      <c r="H10" s="95">
+      <c r="H10" s="43">
         <f>SCHEDE!D38</f>
         <v>0</v>
       </c>
-      <c r="I10" s="96">
+      <c r="I10" s="44">
         <f>SCHEDE!B31</f>
         <v>0</v>
       </c>
@@ -2623,8 +2885,8 @@
       <c r="L10" s="19"/>
       <c r="M10" s="19"/>
       <c r="N10" s="19"/>
-      <c r="O10" s="109"/>
-      <c r="P10" s="110"/>
+      <c r="O10" s="105"/>
+      <c r="P10" s="106"/>
       <c r="Q10" s="18"/>
       <c r="R10" s="20"/>
       <c r="S10" s="20">
@@ -2655,40 +2917,40 @@
       </c>
       <c r="Z10" s="25"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A11" s="98">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A11" s="46">
         <f>SCHEDE!B47</f>
         <v>0</v>
       </c>
-      <c r="B11" s="93">
+      <c r="B11" s="41">
         <f>SCHEDE!D53</f>
         <v>0</v>
       </c>
-      <c r="C11" s="93">
+      <c r="C11" s="41">
         <f>SCHEDE!D55</f>
         <v>0</v>
       </c>
-      <c r="D11" s="93">
+      <c r="D11" s="41">
         <f>SCHEDE!D59</f>
         <v>0</v>
       </c>
-      <c r="E11" s="93">
+      <c r="E11" s="41">
         <f>SCHEDE!B61</f>
         <v>0</v>
       </c>
-      <c r="F11" s="97">
+      <c r="F11" s="45">
         <f>SCHEDE!C61</f>
         <v>0</v>
       </c>
-      <c r="G11" s="94">
+      <c r="G11" s="42">
         <f>SCHEDE!C57</f>
         <v>0</v>
       </c>
-      <c r="H11" s="95">
+      <c r="H11" s="43">
         <f>SCHEDE!D61</f>
         <v>0</v>
       </c>
-      <c r="I11" s="96">
+      <c r="I11" s="44">
         <f>SCHEDE!B54</f>
         <v>0</v>
       </c>
@@ -2696,8 +2958,8 @@
       <c r="L11" s="19"/>
       <c r="M11" s="19"/>
       <c r="N11" s="19"/>
-      <c r="O11" s="109"/>
-      <c r="P11" s="110"/>
+      <c r="O11" s="105"/>
+      <c r="P11" s="106"/>
       <c r="Q11" s="18"/>
       <c r="R11" s="20"/>
       <c r="S11" s="20">
@@ -2728,40 +2990,40 @@
       </c>
       <c r="Z11" s="25"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A12" s="98">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A12" s="46">
         <f>SCHEDE!B70</f>
         <v>0</v>
       </c>
-      <c r="B12" s="93">
+      <c r="B12" s="41">
         <f>SCHEDE!D76</f>
         <v>0</v>
       </c>
-      <c r="C12" s="93">
+      <c r="C12" s="41">
         <f>SCHEDE!D78</f>
         <v>0</v>
       </c>
-      <c r="D12" s="93">
+      <c r="D12" s="41">
         <f>SCHEDE!D82</f>
         <v>0</v>
       </c>
-      <c r="E12" s="93">
+      <c r="E12" s="41">
         <f>SCHEDE!B84</f>
         <v>0</v>
       </c>
-      <c r="F12" s="97">
+      <c r="F12" s="45">
         <f>SCHEDE!C84</f>
         <v>0</v>
       </c>
-      <c r="G12" s="94">
+      <c r="G12" s="42">
         <f>SCHEDE!C80</f>
         <v>0</v>
       </c>
-      <c r="H12" s="95">
+      <c r="H12" s="43">
         <f>SCHEDE!D84</f>
         <v>0</v>
       </c>
-      <c r="I12" s="96">
+      <c r="I12" s="44">
         <f>SCHEDE!B77</f>
         <v>0</v>
       </c>
@@ -2769,8 +3031,8 @@
       <c r="L12" s="19"/>
       <c r="M12" s="19"/>
       <c r="N12" s="19"/>
-      <c r="O12" s="109"/>
-      <c r="P12" s="110"/>
+      <c r="O12" s="105"/>
+      <c r="P12" s="106"/>
       <c r="Q12" s="18"/>
       <c r="R12" s="20"/>
       <c r="S12" s="20">
@@ -2801,13 +3063,13 @@
       </c>
       <c r="Z12" s="25"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="K13" s="18"/>
       <c r="L13" s="19"/>
       <c r="M13" s="19"/>
       <c r="N13" s="19"/>
-      <c r="O13" s="109"/>
-      <c r="P13" s="110"/>
+      <c r="O13" s="105"/>
+      <c r="P13" s="106"/>
       <c r="Q13" s="18"/>
       <c r="R13" s="20"/>
       <c r="S13" s="20">
@@ -2838,13 +3100,13 @@
       </c>
       <c r="Z13" s="25"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="K14" s="18"/>
       <c r="L14" s="19"/>
       <c r="M14" s="19"/>
       <c r="N14" s="19"/>
-      <c r="O14" s="109"/>
-      <c r="P14" s="110"/>
+      <c r="O14" s="105"/>
+      <c r="P14" s="106"/>
       <c r="Q14" s="18"/>
       <c r="R14" s="20"/>
       <c r="S14" s="20">
@@ -2875,13 +3137,13 @@
       </c>
       <c r="Z14" s="25"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="K15" s="18"/>
       <c r="L15" s="19"/>
       <c r="M15" s="19"/>
       <c r="N15" s="19"/>
-      <c r="O15" s="109"/>
-      <c r="P15" s="110"/>
+      <c r="O15" s="105"/>
+      <c r="P15" s="106"/>
       <c r="Q15" s="18"/>
       <c r="R15" s="20"/>
       <c r="S15" s="20">
@@ -2912,13 +3174,13 @@
       </c>
       <c r="Z15" s="25"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="K16" s="18"/>
       <c r="L16" s="19"/>
       <c r="M16" s="19"/>
       <c r="N16" s="19"/>
-      <c r="O16" s="109"/>
-      <c r="P16" s="110"/>
+      <c r="O16" s="105"/>
+      <c r="P16" s="106"/>
       <c r="Q16" s="18"/>
       <c r="R16" s="20"/>
       <c r="S16" s="20">
@@ -2949,13 +3211,13 @@
       </c>
       <c r="Z16" s="25"/>
     </row>
-    <row r="17" spans="11:26" x14ac:dyDescent="0.2">
+    <row r="17" spans="11:26" x14ac:dyDescent="0.25">
       <c r="K17" s="18"/>
       <c r="L17" s="19"/>
       <c r="M17" s="19"/>
       <c r="N17" s="19"/>
-      <c r="O17" s="109"/>
-      <c r="P17" s="110"/>
+      <c r="O17" s="105"/>
+      <c r="P17" s="106"/>
       <c r="Q17" s="18"/>
       <c r="R17" s="20"/>
       <c r="S17" s="20">
@@ -2986,13 +3248,13 @@
       </c>
       <c r="Z17" s="25"/>
     </row>
-    <row r="18" spans="11:26" x14ac:dyDescent="0.2">
+    <row r="18" spans="11:26" x14ac:dyDescent="0.25">
       <c r="K18" s="18"/>
       <c r="L18" s="19"/>
       <c r="M18" s="19"/>
       <c r="N18" s="19"/>
-      <c r="O18" s="109"/>
-      <c r="P18" s="110"/>
+      <c r="O18" s="105"/>
+      <c r="P18" s="106"/>
       <c r="Q18" s="18"/>
       <c r="R18" s="20"/>
       <c r="S18" s="20">
@@ -3023,13 +3285,13 @@
       </c>
       <c r="Z18" s="25"/>
     </row>
-    <row r="19" spans="11:26" x14ac:dyDescent="0.2">
+    <row r="19" spans="11:26" x14ac:dyDescent="0.25">
       <c r="K19" s="18"/>
       <c r="L19" s="19"/>
       <c r="M19" s="19"/>
       <c r="N19" s="19"/>
-      <c r="O19" s="109"/>
-      <c r="P19" s="110"/>
+      <c r="O19" s="105"/>
+      <c r="P19" s="106"/>
       <c r="Q19" s="18"/>
       <c r="R19" s="20"/>
       <c r="S19" s="20">
@@ -3060,13 +3322,13 @@
       </c>
       <c r="Z19" s="25"/>
     </row>
-    <row r="20" spans="11:26" x14ac:dyDescent="0.2">
+    <row r="20" spans="11:26" x14ac:dyDescent="0.25">
       <c r="K20" s="18"/>
       <c r="L20" s="19"/>
       <c r="M20" s="19"/>
       <c r="N20" s="19"/>
-      <c r="O20" s="109"/>
-      <c r="P20" s="110"/>
+      <c r="O20" s="105"/>
+      <c r="P20" s="106"/>
       <c r="Q20" s="18"/>
       <c r="R20" s="20"/>
       <c r="S20" s="20">
@@ -3097,13 +3359,13 @@
       </c>
       <c r="Z20" s="25"/>
     </row>
-    <row r="21" spans="11:26" x14ac:dyDescent="0.2">
+    <row r="21" spans="11:26" x14ac:dyDescent="0.25">
       <c r="K21" s="18"/>
       <c r="L21" s="19"/>
       <c r="M21" s="19"/>
       <c r="N21" s="19"/>
-      <c r="O21" s="109"/>
-      <c r="P21" s="110"/>
+      <c r="O21" s="105"/>
+      <c r="P21" s="106"/>
       <c r="Q21" s="18"/>
       <c r="R21" s="20"/>
       <c r="S21" s="20">
@@ -3134,13 +3396,13 @@
       </c>
       <c r="Z21" s="25"/>
     </row>
-    <row r="22" spans="11:26" x14ac:dyDescent="0.2">
+    <row r="22" spans="11:26" x14ac:dyDescent="0.25">
       <c r="K22" s="18"/>
       <c r="L22" s="19"/>
       <c r="M22" s="19"/>
       <c r="N22" s="19"/>
-      <c r="O22" s="109"/>
-      <c r="P22" s="110"/>
+      <c r="O22" s="105"/>
+      <c r="P22" s="106"/>
       <c r="Q22" s="18"/>
       <c r="R22" s="20"/>
       <c r="S22" s="20">
@@ -3171,13 +3433,13 @@
       </c>
       <c r="Z22" s="25"/>
     </row>
-    <row r="23" spans="11:26" x14ac:dyDescent="0.2">
+    <row r="23" spans="11:26" x14ac:dyDescent="0.25">
       <c r="K23" s="18"/>
       <c r="L23" s="19"/>
       <c r="M23" s="19"/>
       <c r="N23" s="19"/>
-      <c r="O23" s="109"/>
-      <c r="P23" s="110"/>
+      <c r="O23" s="105"/>
+      <c r="P23" s="106"/>
       <c r="Q23" s="18"/>
       <c r="R23" s="20"/>
       <c r="S23" s="20">
@@ -3208,13 +3470,13 @@
       </c>
       <c r="Z23" s="25"/>
     </row>
-    <row r="24" spans="11:26" x14ac:dyDescent="0.2">
+    <row r="24" spans="11:26" x14ac:dyDescent="0.25">
       <c r="K24" s="18"/>
       <c r="L24" s="19"/>
       <c r="M24" s="19"/>
       <c r="N24" s="19"/>
-      <c r="O24" s="109"/>
-      <c r="P24" s="110"/>
+      <c r="O24" s="105"/>
+      <c r="P24" s="106"/>
       <c r="Q24" s="18"/>
       <c r="R24" s="20"/>
       <c r="S24" s="20">
@@ -3245,13 +3507,13 @@
       </c>
       <c r="Z24" s="25"/>
     </row>
-    <row r="25" spans="11:26" x14ac:dyDescent="0.2">
+    <row r="25" spans="11:26" x14ac:dyDescent="0.25">
       <c r="K25" s="18"/>
       <c r="L25" s="19"/>
       <c r="M25" s="19"/>
       <c r="N25" s="19"/>
-      <c r="O25" s="109"/>
-      <c r="P25" s="110"/>
+      <c r="O25" s="105"/>
+      <c r="P25" s="106"/>
       <c r="Q25" s="18"/>
       <c r="R25" s="20"/>
       <c r="S25" s="20">
@@ -3282,13 +3544,13 @@
       </c>
       <c r="Z25" s="25"/>
     </row>
-    <row r="26" spans="11:26" x14ac:dyDescent="0.2">
+    <row r="26" spans="11:26" x14ac:dyDescent="0.25">
       <c r="K26" s="18"/>
       <c r="L26" s="19"/>
       <c r="M26" s="19"/>
       <c r="N26" s="19"/>
-      <c r="O26" s="119"/>
-      <c r="P26" s="120"/>
+      <c r="O26" s="115"/>
+      <c r="P26" s="116"/>
       <c r="Q26" s="18"/>
       <c r="R26" s="20"/>
       <c r="S26" s="20">
@@ -3319,13 +3581,13 @@
       </c>
       <c r="Z26" s="25"/>
     </row>
-    <row r="27" spans="11:26" x14ac:dyDescent="0.2">
+    <row r="27" spans="11:26" x14ac:dyDescent="0.25">
       <c r="K27" s="18"/>
       <c r="L27" s="19"/>
       <c r="M27" s="19"/>
       <c r="N27" s="19"/>
-      <c r="O27" s="119"/>
-      <c r="P27" s="120"/>
+      <c r="O27" s="115"/>
+      <c r="P27" s="116"/>
       <c r="Q27" s="18"/>
       <c r="R27" s="20"/>
       <c r="S27" s="20">
@@ -3356,13 +3618,13 @@
       </c>
       <c r="Z27" s="25"/>
     </row>
-    <row r="28" spans="11:26" x14ac:dyDescent="0.2">
+    <row r="28" spans="11:26" x14ac:dyDescent="0.25">
       <c r="K28" s="26"/>
       <c r="L28" s="26"/>
       <c r="M28" s="26"/>
       <c r="N28" s="27"/>
-      <c r="O28" s="119"/>
-      <c r="P28" s="120"/>
+      <c r="O28" s="115"/>
+      <c r="P28" s="116"/>
       <c r="Q28" s="18"/>
       <c r="R28" s="20"/>
       <c r="S28" s="20">
@@ -3393,13 +3655,13 @@
       </c>
       <c r="Z28" s="25"/>
     </row>
-    <row r="29" spans="11:26" x14ac:dyDescent="0.2">
+    <row r="29" spans="11:26" x14ac:dyDescent="0.25">
       <c r="K29" s="26"/>
       <c r="L29" s="26"/>
       <c r="M29" s="26"/>
       <c r="N29" s="27"/>
-      <c r="O29" s="119"/>
-      <c r="P29" s="120"/>
+      <c r="O29" s="115"/>
+      <c r="P29" s="116"/>
       <c r="Q29" s="18"/>
       <c r="R29" s="20"/>
       <c r="S29" s="20">
@@ -3430,13 +3692,13 @@
       </c>
       <c r="Z29" s="25"/>
     </row>
-    <row r="30" spans="11:26" x14ac:dyDescent="0.2">
+    <row r="30" spans="11:26" x14ac:dyDescent="0.25">
       <c r="K30" s="26"/>
       <c r="L30" s="26"/>
       <c r="M30" s="26"/>
       <c r="N30" s="27"/>
-      <c r="O30" s="119"/>
-      <c r="P30" s="120"/>
+      <c r="O30" s="115"/>
+      <c r="P30" s="116"/>
       <c r="Q30" s="18"/>
       <c r="R30" s="20"/>
       <c r="S30" s="20">
@@ -3467,13 +3729,13 @@
       </c>
       <c r="Z30" s="25"/>
     </row>
-    <row r="31" spans="11:26" x14ac:dyDescent="0.2">
+    <row r="31" spans="11:26" x14ac:dyDescent="0.25">
       <c r="K31" s="26"/>
       <c r="L31" s="26"/>
       <c r="M31" s="26"/>
       <c r="N31" s="27"/>
-      <c r="O31" s="119"/>
-      <c r="P31" s="120"/>
+      <c r="O31" s="115"/>
+      <c r="P31" s="116"/>
       <c r="Q31" s="18"/>
       <c r="R31" s="20"/>
       <c r="S31" s="20">
@@ -3504,13 +3766,13 @@
       </c>
       <c r="Z31" s="25"/>
     </row>
-    <row r="32" spans="11:26" x14ac:dyDescent="0.2">
+    <row r="32" spans="11:26" x14ac:dyDescent="0.25">
       <c r="K32" s="26"/>
       <c r="L32" s="26"/>
       <c r="M32" s="26"/>
       <c r="N32" s="27"/>
-      <c r="O32" s="119"/>
-      <c r="P32" s="120"/>
+      <c r="O32" s="115"/>
+      <c r="P32" s="116"/>
       <c r="Q32" s="18"/>
       <c r="R32" s="20"/>
       <c r="S32" s="20">
@@ -3541,13 +3803,13 @@
       </c>
       <c r="Z32" s="25"/>
     </row>
-    <row r="33" spans="11:26" x14ac:dyDescent="0.2">
+    <row r="33" spans="11:26" x14ac:dyDescent="0.25">
       <c r="K33" s="26"/>
       <c r="L33" s="26"/>
       <c r="M33" s="26"/>
       <c r="N33" s="27"/>
-      <c r="O33" s="119"/>
-      <c r="P33" s="120"/>
+      <c r="O33" s="115"/>
+      <c r="P33" s="116"/>
       <c r="Q33" s="18"/>
       <c r="R33" s="20"/>
       <c r="S33" s="20">
@@ -3578,13 +3840,13 @@
       </c>
       <c r="Z33" s="25"/>
     </row>
-    <row r="34" spans="11:26" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="11:26" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K34" s="26"/>
       <c r="L34" s="26"/>
       <c r="M34" s="26"/>
       <c r="N34" s="27"/>
-      <c r="O34" s="119"/>
-      <c r="P34" s="120"/>
+      <c r="O34" s="115"/>
+      <c r="P34" s="116"/>
       <c r="Q34" s="18"/>
       <c r="R34" s="20"/>
       <c r="S34" s="20">
@@ -3615,7 +3877,7 @@
       </c>
       <c r="Z34" s="29"/>
     </row>
-    <row r="35" spans="11:26" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="11:26" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L35" s="30"/>
       <c r="M35" s="30"/>
       <c r="N35" s="30"/>

</xml_diff>